<commit_message>
updated tabulation script and added some output scripts
</commit_message>
<xml_diff>
--- a/templates/chapter3.xlsx
+++ b/templates/chapter3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\crvs_report\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C2522CB-0B60-4EFC-ABFC-F765A8E8A8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E12FC35-6897-4B7E-9A0A-D6712B84243D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FB2C1DD-F60E-43CB-80FB-5A040F5AF174}"/>
+    <workbookView xWindow="1650" yWindow="1860" windowWidth="24150" windowHeight="11610" firstSheet="2" activeTab="10" xr2:uid="{9FB2C1DD-F60E-43CB-80FB-5A040F5AF174}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 3.1" sheetId="1" r:id="rId1"/>
@@ -988,7 +988,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -999,26 +999,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1032,6 +1014,34 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1346,28 +1356,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24092F0A-1B12-4750-ACF1-C738CAB357F4}">
-  <dimension ref="B1:F7"/>
+  <dimension ref="B1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="12"/>
+    </row>
+    <row r="3" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="10"/>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1380,8 +1410,26 @@
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+    </row>
+    <row r="4" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1389,8 +1437,26 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+    </row>
+    <row r="5" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1398,8 +1464,26 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+    </row>
+    <row r="6" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1407,8 +1491,26 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+    </row>
+    <row r="7" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1416,13 +1518,26 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1432,46 +1547,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80C5757-6D9C-46E8-BEBF-D77CA1FBCFFE}">
   <dimension ref="B1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="8"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="2:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1480,63 +1597,57 @@
         <v>32</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="12"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="12"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="12"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="12"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="12"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="12"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="12"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="12"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="12"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="12"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="12"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="12"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="12"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="12"/>
+      <c r="H8" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1545,32 +1656,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11B39783-B519-46B4-A9A8-DC793268522E}">
   <dimension ref="B1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1580,7 +1693,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="12"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -1588,7 +1701,7 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -1596,7 +1709,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="12"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
@@ -1604,7 +1717,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="12"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -1612,7 +1725,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="12"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
@@ -1620,7 +1733,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="12"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
@@ -1628,7 +1741,7 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="12"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
@@ -1636,7 +1749,7 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="12"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
@@ -1644,7 +1757,7 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="12"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
@@ -1654,7 +1767,7 @@
       <c r="D13" s="3">
         <v>0</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1666,13 +1779,9 @@
       <c r="D14" s="3">
         <v>100</v>
       </c>
-      <c r="E14" s="12"/>
+      <c r="E14" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1681,33 +1790,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47ECDD77-11CD-4E16-9A5F-32144D6C1E55}">
   <dimension ref="B1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:K3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="7" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="7" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="8"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="12"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
@@ -2025,12 +2136,6 @@
       <c r="K23" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2039,25 +2144,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{038B50A1-2A40-4360-9D85-27A0120E48B5}">
   <dimension ref="B1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="8"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
@@ -2135,10 +2242,6 @@
       <c r="G9" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:G2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2147,25 +2250,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{183EE185-D4F9-4D58-A34A-BA6F522CE730}">
   <dimension ref="B1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="8"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
@@ -2243,46 +2348,44 @@
       <c r="G9" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:G2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{965EB52F-BC1D-4990-BA08-CF6446065F45}">
-  <dimension ref="B1:L9"/>
+  <dimension ref="B1:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="7" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="7" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="9"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="4"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
@@ -2310,140 +2413,316 @@
       <c r="K3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="9"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="9"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="9"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="9"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="9"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="9"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="9"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="16"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="16"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="16"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="16"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="16"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="16"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="16"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="16"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="16"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="16"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="16"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB65BB3-6EC5-4AF8-BA2D-D8915652CCFA}">
-  <dimension ref="B1:K9"/>
+  <dimension ref="B1:K40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="7" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="7" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="8"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="12"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
@@ -2476,100 +2755,466 @@
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="16"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="16"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="16"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="16"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="16"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="16"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="16"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="16"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="16"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="16"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="16"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="16"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="16"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="16"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="16"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="16"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="16"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="16"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="16"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="16"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="16"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="16"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="16"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="16"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="16"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="16"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="16"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="16"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C620816-95D3-4822-9952-F0112282B561}">
-  <dimension ref="B1:L9"/>
+  <dimension ref="B1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2577,28 +3222,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="7" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="7" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="9"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="4"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
@@ -2626,140 +3271,376 @@
       <c r="K3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="9"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="9"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="9"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="9"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="9"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="9"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="9"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="16"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="16"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="16"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="16"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="16"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="16"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="16"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="16"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="16"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="16"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="16"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="16"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="16"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="16"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="16"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="16"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="16"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC924658-72C0-4335-B536-CF503B84ADD6}">
-  <dimension ref="B1:K9"/>
+  <dimension ref="B1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:K25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="7" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="7" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="8"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="12"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
@@ -2792,141 +3673,327 @@
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="16"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="16"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="16"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="16"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="16"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="16"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="16"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="16"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="16"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="16"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="16"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="16"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="16"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080C2BC6-5D59-4560-AB3D-A5EA86FC43F8}">
-  <dimension ref="B1:H9"/>
+  <dimension ref="B1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="8"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="2:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="5" t="s">
         <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2935,122 +4002,244 @@
         <v>21</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="12"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="12"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="12"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="12"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="12"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="12"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="12"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="12"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="12"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="12"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="12"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="12"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="12"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="12"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="12"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="12"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="12"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="16"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="16"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="16"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="16"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="16"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="16"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="16"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="16"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="16"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="16"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="16"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E61F891-009A-4B18-9888-792E47049795}">
-  <dimension ref="B1:H9"/>
+  <dimension ref="B1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:H24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="8"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="2:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3059,74 +4248,203 @@
         <v>21</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="12"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="12"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="12"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="12"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="12"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="12"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="12"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="12"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="12"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="12"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="12"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="12"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="12"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="12"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="12"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="12"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="12"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="16"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="16"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="16"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="16"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="16"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="16"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="16"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="16"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="16"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="16"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="16"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="16"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>